<commit_message>
N4_EB, N5, N6, RH7 points files done
</commit_message>
<xml_diff>
--- a/data4_found_points/zivid_frames.xlsx
+++ b/data4_found_points/zivid_frames.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edvardbruun/Documents/GitHub/zivid_camera/data4_found_points/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edvard\Documents\GitHub\zivid_camera\data4_found_points\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D09498-71CA-C34E-8F87-0E82F60F69E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29C1098-A243-4E0F-93FB-D55B77FED00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1060" windowWidth="30240" windowHeight="17440" xr2:uid="{EC091DB4-3700-8243-BAF1-3D0CCA7A1FD4}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{EC091DB4-3700-8243-BAF1-3D0CCA7A1FD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>N3</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>unload</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -277,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -297,6 +300,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -304,75 +373,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -689,289 +689,298 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5663E4B-AC02-B248-9E88-3A5760C4F0E0}">
-  <dimension ref="A2:M10"/>
+  <dimension ref="A2:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.125" bestFit="1" customWidth="1"/>
     <col min="4" max="11" width="4.5" customWidth="1"/>
-    <col min="12" max="12" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="7" t="s">
+    <row r="2" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="9"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="31"/>
     </row>
-    <row r="4" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="27">
-        <v>0</v>
-      </c>
-      <c r="E4" s="28">
+      <c r="D4" s="23">
+        <v>0</v>
+      </c>
+      <c r="E4" s="24">
         <v>0.125</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="24">
         <v>0.25</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="24">
         <f>E4*3</f>
         <v>0.375</v>
       </c>
-      <c r="H4" s="27">
+      <c r="H4" s="23">
         <v>0.5</v>
       </c>
-      <c r="I4" s="28">
+      <c r="I4" s="24">
         <f>E4*5</f>
         <v>0.625</v>
       </c>
-      <c r="J4" s="28">
+      <c r="J4" s="24">
         <v>0.75</v>
       </c>
-      <c r="K4" s="28">
+      <c r="K4" s="24">
         <f>E4*7</f>
         <v>0.875</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="8">
         <v>1</v>
       </c>
-      <c r="M4" s="32" t="s">
+      <c r="M4" s="28" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="14">
-        <v>0</v>
-      </c>
-      <c r="C5" s="22">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="11">
+        <v>0</v>
+      </c>
+      <c r="C5" s="18">
         <v>25</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="25">
         <f>ROUND(($C5-1)*D$4,0)</f>
         <v>0</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15">
+      <c r="E5" s="12"/>
+      <c r="F5" s="12">
         <f>ROUND(($C5-1)*F$4,0)</f>
         <v>6</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15">
+      <c r="G5" s="12"/>
+      <c r="H5" s="12">
         <f>ROUND(($C5-1)*H$4,0)</f>
         <v>12</v>
       </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15">
+      <c r="I5" s="12"/>
+      <c r="J5" s="12">
         <f>ROUND(($C5-1)*J$4,0)</f>
         <v>18</v>
       </c>
-      <c r="K5" s="15"/>
-      <c r="L5" s="16">
+      <c r="K5" s="12"/>
+      <c r="L5" s="13">
         <f>ROUND(($C5-1)*L$4,0)</f>
         <v>24</v>
       </c>
-      <c r="M5" s="23">
+      <c r="M5" s="19">
         <f>C5</f>
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="10">
-        <v>0</v>
-      </c>
-      <c r="C6" s="26">
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+      <c r="C6" s="22">
         <v>37</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="26">
         <f>ROUND(($C6-1)*D$4,0)</f>
         <v>0</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="15">
         <f>ROUND(($C6-1)*E$4,0)</f>
         <v>5</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="15">
         <f t="shared" ref="F6:L6" si="0">ROUND(($C6-1)*F$4,0)</f>
         <v>9</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="15">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="15">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="15">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="K6" s="19">
+      <c r="K6" s="15">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="L6" s="20">
+      <c r="L6" s="16">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="M6" s="23">
+      <c r="M6" s="19">
         <f t="shared" ref="M6:M9" si="1">C6</f>
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="18">
-        <v>0</v>
-      </c>
-      <c r="C7" s="23">
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="19">
         <v>37</v>
       </c>
-      <c r="D7" s="30">
-        <f t="shared" ref="D6:D9" si="2">ROUND(($C7-1)*D$4,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19">
-        <f t="shared" ref="F6:F9" si="3">ROUND(($C7-1)*F$4,0)</f>
+      <c r="D7" s="26">
+        <f t="shared" ref="D7:D9" si="2">ROUND(($C7-1)*D$4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15">
+        <f t="shared" ref="F7:F9" si="3">ROUND(($C7-1)*F$4,0)</f>
         <v>9</v>
       </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19">
-        <f t="shared" ref="H6:H9" si="4">ROUND(($C7-1)*H$4,0)</f>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15">
+        <f t="shared" ref="H7:H9" si="4">ROUND(($C7-1)*H$4,0)</f>
         <v>18</v>
       </c>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19">
-        <f t="shared" ref="J6:J9" si="5">ROUND(($C7-1)*J$4,0)</f>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15">
+        <f t="shared" ref="J7:J9" si="5">ROUND(($C7-1)*J$4,0)</f>
         <v>27</v>
       </c>
-      <c r="K7" s="19"/>
-      <c r="L7" s="20">
-        <f t="shared" ref="L6:L9" si="6">ROUND(($C7-1)*L$4,0)</f>
+      <c r="K7" s="15"/>
+      <c r="L7" s="16">
+        <f t="shared" ref="L7:L9" si="6">ROUND(($C7-1)*L$4,0)</f>
         <v>36</v>
       </c>
-      <c r="M7" s="23">
+      <c r="M7" s="19">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
+      <c r="N7" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="18">
-        <v>0</v>
-      </c>
-      <c r="C8" s="23">
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="19">
         <v>27</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="26">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19">
+      <c r="E8" s="15"/>
+      <c r="F8" s="15">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19">
+      <c r="G8" s="15"/>
+      <c r="H8" s="15">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19">
+      <c r="I8" s="15"/>
+      <c r="J8" s="15">
         <f t="shared" si="5"/>
         <v>20</v>
       </c>
-      <c r="K8" s="19"/>
-      <c r="L8" s="20">
+      <c r="K8" s="15"/>
+      <c r="L8" s="16">
         <f t="shared" si="6"/>
         <v>26</v>
       </c>
-      <c r="M8" s="23">
+      <c r="M8" s="19">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
+      <c r="N8" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="4">
         <v>0</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="20">
         <v>28</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="27">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12">
+      <c r="E9" s="9"/>
+      <c r="F9" s="9">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12">
+      <c r="G9" s="9"/>
+      <c r="H9" s="9">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12">
+      <c r="I9" s="9"/>
+      <c r="J9" s="9">
         <f t="shared" si="5"/>
         <v>20</v>
       </c>
-      <c r="K9" s="12"/>
-      <c r="L9" s="21">
+      <c r="K9" s="9"/>
+      <c r="L9" s="17">
         <f t="shared" si="6"/>
         <v>27</v>
       </c>
-      <c r="M9" s="24">
+      <c r="M9" s="20">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
+      <c r="N9" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>

</xml_diff>